<commit_message>
adjust for order import
</commit_message>
<xml_diff>
--- a/server/resource/excel/template.xlsx
+++ b/server/resource/excel/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xujun/gva/gin-vue-admin/server/resource/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38CDAEC-697E-CB45-B729-DB2C6DA59B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587087E6-D4E4-0949-A7C9-BCAC4F025A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20720" windowHeight="13420" xr2:uid="{C538948F-8F36-444C-A3AB-77126F948885}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13420" xr2:uid="{C538948F-8F36-444C-A3AB-77126F948885}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,6 +277,27 @@
     <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -294,27 +315,6 @@
     </xf>
     <xf numFmtId="178" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,7 +465,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -753,7 +753,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -765,7 +765,7 @@
   <dimension ref="A1:X1252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.83203125" defaultRowHeight="15"/>
@@ -803,203 +803,203 @@
       </c>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="11"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
       <c r="P6" s="13"/>
       <c r="T6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="32"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
       <c r="P7" s="13"/>
       <c r="T7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="33"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33"/>
-      <c r="X7" s="33"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="14"/>
       <c r="T8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="32"/>
-      <c r="X8" s="32"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="30"/>
+      <c r="X8" s="30"/>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
       <c r="P9" s="14"/>
       <c r="T9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U9" s="33"/>
-      <c r="V9" s="33"/>
-      <c r="W9" s="33"/>
-      <c r="X9" s="33"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
       <c r="T10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U10" s="33"/>
-      <c r="V10" s="33"/>
-      <c r="W10" s="33"/>
-      <c r="X10" s="33"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26"/>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:24" s="6" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="34" t="s">
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="30" t="s">
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
       <c r="R13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="S13" s="34" t="s">
+      <c r="S13" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="T13" s="34"/>
-      <c r="U13" s="34" t="s">
+      <c r="T13" s="24"/>
+      <c r="U13" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34" t="s">
+      <c r="V13" s="24"/>
+      <c r="W13" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="X13" s="34"/>
+      <c r="X13" s="24"/>
     </row>
     <row r="14" spans="1:24" s="6" customFormat="1" ht="23.25" customHeight="1">
       <c r="A14" s="8"/>
@@ -1028,30 +1028,30 @@
       <c r="X14" s="9"/>
     </row>
     <row r="15" spans="1:24" s="6" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="29"/>
-      <c r="X15" s="25"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="32"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="32"/>
     </row>
     <row r="16" spans="1:24" s="6" customFormat="1" ht="23.25" customHeight="1">
       <c r="A16" s="8"/>
@@ -21409,18 +21409,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="I12:O12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:K13"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="A6:G7"/>
-    <mergeCell ref="I6:O7"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="U7:X7"/>
-    <mergeCell ref="U8:X8"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="W13:X13"/>
     <mergeCell ref="A8:G9"/>
@@ -21431,6 +21419,18 @@
     <mergeCell ref="I10:O10"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="I11:O11"/>
+    <mergeCell ref="A6:G7"/>
+    <mergeCell ref="I6:O7"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="U8:X8"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="I12:O12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:K13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="O13:Q13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>